<commit_message>
last matrix break fix
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300542.xlsx
+++ b/src/main/resources/SZ300542.xlsx
@@ -68,7 +68,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>309.0</v>
+        <v>346.0</v>
       </c>
     </row>
     <row r="2">
@@ -94,7 +94,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20161111</t>
+          <t>20161122</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -639,6 +639,86 @@
       </c>
       <c r="B58" t="n">
         <v>1358.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>20200812</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1165.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20201013</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2534.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>20210114</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1199.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>20210120</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1403.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>20210208</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1066.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20210302</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1264.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20210315</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1077.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>20210402</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1269.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>